<commit_message>
Arreglo de los roles
</commit_message>
<xml_diff>
--- a/public/import-excel-users/caproin-import-users.xlsx
+++ b/public/import-excel-users/caproin-import-users.xlsx
@@ -238,15 +238,15 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.33"/>
   </cols>
   <sheetData>
@@ -287,7 +287,7 @@
         <v>1601132623</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>

</xml_diff>